<commit_message>
Update Codebook-climate trust variable mappings.xlsx
</commit_message>
<xml_diff>
--- a/Codebook-climate trust variable mappings.xlsx
+++ b/Codebook-climate trust variable mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Dropbox\Climate-Trust-Replication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55956479-1EA0-4FD4-AAF0-515EC07173E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2956B084-34FD-48AB-A340-DD88B131DDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5670" windowWidth="29040" windowHeight="15720" xr2:uid="{E7AB07C1-8825-45AA-A938-29CF9AF9D7AC}"/>
   </bookViews>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">High Trust  Low Trust  Mod Trust </t>
   </si>
   <si>
-    <t>Recode fromk Q41: High Trust(7-10)  Low Trust (4-5)  Mod Trust (4-5)</t>
+    <t>Recode fromk Q41: High Trust(7-10)  Low Trust (0-3)  Mod Trust (4-5)</t>
   </si>
 </sst>
 </file>

</xml_diff>